<commit_message>
Data Driven - Creating Test case and executing it on 10 different nodes
</commit_message>
<xml_diff>
--- a/DataDrivenGrid/src/test/resources/testdata/BankManagerSuite.xlsx
+++ b/DataDrivenGrid/src/test/resources/testdata/BankManagerSuite.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\seleniumworkspaces\LiveProjects\TestDataProject\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\seleniumworkspaces\LiveProjects\DataDrivenGrid\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>TestCases</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>firstname</t>
   </si>
   <si>
@@ -75,22 +72,37 @@
     <t>currency</t>
   </si>
   <si>
-    <t>Raman Arora</t>
-  </si>
-  <si>
-    <t>Rahul Arora</t>
-  </si>
-  <si>
     <t>Rupee</t>
   </si>
   <si>
     <t>Dollar</t>
   </si>
   <si>
-    <t>Amit Kumar</t>
-  </si>
-  <si>
-    <t>Abhigya</t>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Harry Potter</t>
+  </si>
+  <si>
+    <t>Ron Weasly</t>
+  </si>
+  <si>
+    <t>Hermoine Granger</t>
+  </si>
+  <si>
+    <t>Pound</t>
   </si>
 </sst>
 </file>
@@ -410,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,119 +459,146 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>